<commit_message>
Change to Selenium Grid
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_Data.xlsx
+++ b/src/test/resources/Test_Data.xlsx
@@ -1,3 +1,448 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr documentId="10_ncr:8100000_{6C6EC5AC-ECBB-4307-B635-86A4C4C52888}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <bookViews>
+    <workbookView activeTab="1" windowHeight="12645" windowWidth="22260" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Testdata" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
+  </sheets>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+  <si>
+    <t>Sl.No</t>
+  </si>
+  <si>
+    <t>TEST_CASE_ID</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Search Term</t>
+  </si>
+  <si>
+    <t>TC_01</t>
+  </si>
+  <si>
+    <t>TC_02</t>
+  </si>
+  <si>
+    <t>TC_03</t>
+  </si>
+  <si>
+    <t>TC_04</t>
+  </si>
+  <si>
+    <t>http://www.google.com</t>
+  </si>
+  <si>
+    <t>http://www.yahoo.com</t>
+  </si>
+  <si>
+    <t>http://www.bing.com</t>
+  </si>
+  <si>
+    <t>http://www.google.in</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>TC01_01</t>
+  </si>
+  <si>
+    <t>TC01_02</t>
+  </si>
+  <si>
+    <t>TC01_03</t>
+  </si>
+  <si>
+    <t>TC01_04</t>
+  </si>
+  <si>
+    <t>http://microsoft.com</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="3">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+  </fills>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr lastClr="000000" val="windowText"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -145,7 +590,9 @@
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
@@ -169,9 +616,7 @@
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>